<commit_message>
modified template for last cell
</commit_message>
<xml_diff>
--- a/excelgen/src/main/resources/person_template_address.xlsx
+++ b/excelgen/src/main/resources/person_template_address.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u725561\excel-templating\excelgen\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63CB9370-7247-4A89-A455-70621AC8A0AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69D6003-A437-4FDA-BFEE-68E1A580091F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,12 +42,29 @@
         </r>
       </text>
     </comment>
+    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{1857C3B0-97B5-4FFB-ACEB-0154E3CCEE3F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>JXLS Command:
+This row contains the jx:if condition.
+If condition is true, the next row(s) will be included.
+If false, they will be removed from output.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Person Report</t>
   </si>
@@ -64,13 +81,22 @@
     <t>${person.age}</t>
   </si>
   <si>
-    <t>jx:if(condition="person.age &lt; 18", lastCell="B6")</t>
-  </si>
-  <si>
     <t>Parent:</t>
   </si>
   <si>
     <t>${person.parentName}</t>
+  </si>
+  <si>
+    <t>Address:</t>
+  </si>
+  <si>
+    <t>${person.address.addressLine}</t>
+  </si>
+  <si>
+    <t>jx:if(condition="person.age &lt; 18", lastCell="A6")</t>
+  </si>
+  <si>
+    <t>jx:if(condition="person.addressExists ", lastCell="A9")</t>
   </si>
 </sst>
 </file>
@@ -454,15 +480,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="44.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -489,15 +515,28 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>